<commit_message>
Updates to inclusion - linked tables
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKHOUSEHOLD/Forms/MASKHOUSEHOLD/MASKHOUSEHOLD.xlsx
+++ b/app/config/tables/MASKHOUSEHOLD/Forms/MASKHOUSEHOLD/MASKHOUSEHOLD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8178BC6D-512F-4481-A090-8AA65BE75D73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7334B2AD-D2FF-46F5-A68F-9A5DA04084D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,9 +11,10 @@
     <sheet name="settings" sheetId="1" r:id="rId1"/>
     <sheet name="survey" sheetId="12" r:id="rId2"/>
     <sheet name="choices" sheetId="3" r:id="rId3"/>
-    <sheet name="calculates" sheetId="7" r:id="rId4"/>
-    <sheet name="prompt_types" sheetId="6" r:id="rId5"/>
-    <sheet name="model" sheetId="4" r:id="rId6"/>
+    <sheet name="queries" sheetId="13" r:id="rId4"/>
+    <sheet name="model" sheetId="4" r:id="rId5"/>
+    <sheet name="calculates" sheetId="7" r:id="rId6"/>
+    <sheet name="prompt_types" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="150">
   <si>
     <t>setting_name</t>
   </si>
@@ -398,13 +399,91 @@
     <t>grupo</t>
   </si>
   <si>
-    <t>name of family</t>
-  </si>
-  <si>
     <t>family</t>
   </si>
   <si>
     <t>grupo de estudio</t>
+  </si>
+  <si>
+    <t>TABZ</t>
+  </si>
+  <si>
+    <t>CAMO</t>
+  </si>
+  <si>
+    <t>FAM</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Other variables</t>
+  </si>
+  <si>
+    <t>Randomization variable</t>
+  </si>
+  <si>
+    <t>HOUSEGRP</t>
+  </si>
+  <si>
+    <t>HHOID</t>
+  </si>
+  <si>
+    <t>BAIRRO</t>
+  </si>
+  <si>
+    <t>RANGROUP</t>
+  </si>
+  <si>
+    <t>query_name</t>
+  </si>
+  <si>
+    <t>query_type</t>
+  </si>
+  <si>
+    <t>linked_form_id</t>
+  </si>
+  <si>
+    <t>linked_table_id</t>
+  </si>
+  <si>
+    <t>selection</t>
+  </si>
+  <si>
+    <t>selectionArgs</t>
+  </si>
+  <si>
+    <t>newRowInitialElementKeyToValueMap</t>
+  </si>
+  <si>
+    <t>openRowInitialElementKeyToValueMap</t>
+  </si>
+  <si>
+    <t>linked_table</t>
+  </si>
+  <si>
+    <t>persons</t>
+  </si>
+  <si>
+    <t>HHOID = ?</t>
+  </si>
+  <si>
+    <t>[data('HHOID')]</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>MASKINCL</t>
+  </si>
+  <si>
+    <t>display.hide_delete_button</t>
+  </si>
+  <si>
+    <t>display.hide_add_instance</t>
   </si>
 </sst>
 </file>
@@ -501,7 +580,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -522,6 +601,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -919,11 +1000,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,9 +1022,11 @@
     <col min="11" max="11" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
@@ -983,13 +1066,19 @@
       <c r="M1" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>46</v>
       </c>
@@ -1000,7 +1089,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>46</v>
       </c>
@@ -1011,7 +1100,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>46</v>
       </c>
@@ -1022,198 +1111,196 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" t="s">
-        <v>123</v>
-      </c>
-      <c r="H8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" t="s">
+        <v>114</v>
+      </c>
+      <c r="H14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H17" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>49</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="G18" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="G19" t="s">
-        <v>113</v>
-      </c>
-      <c r="H19" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>46</v>
-      </c>
-      <c r="G22" t="s">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" t="s">
+        <v>143</v>
+      </c>
+      <c r="G21" t="s">
         <v>50</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="N21" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1889,6 +1976,301 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFE3BA1-1F6C-49DE-9395-0B7AA4A723B3}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView zoomScale="94" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="10"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I8:I24">
+    <sortCondition ref="I8"/>
+  </sortState>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1933,7 +2315,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1982,45 +2364,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView zoomScale="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D83"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:C35">
-    <sortCondition ref="A21"/>
-  </sortState>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to survey and logic before field test
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKHOUSEHOLD/Forms/MASKHOUSEHOLD/MASKHOUSEHOLD.xlsx
+++ b/app/config/tables/MASKHOUSEHOLD/Forms/MASKHOUSEHOLD/MASKHOUSEHOLD.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79CDA4F-4DFE-4CFE-BBFB-F44766B240C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B9A3CC-8DBA-41D5-820B-8D496B0FEADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="163">
   <si>
     <t>setting_name</t>
   </si>
@@ -186,9 +186,6 @@
     <t>select_one</t>
   </si>
   <si>
-    <t>linked table</t>
-  </si>
-  <si>
     <t>DATEX</t>
   </si>
   <si>
@@ -390,21 +387,6 @@
     <t>What is the water source?</t>
   </si>
   <si>
-    <t>tabz</t>
-  </si>
-  <si>
-    <t>camo</t>
-  </si>
-  <si>
-    <t>grupo</t>
-  </si>
-  <si>
-    <t>family</t>
-  </si>
-  <si>
-    <t>grupo de estudio</t>
-  </si>
-  <si>
     <t>TABZ</t>
   </si>
   <si>
@@ -490,6 +472,57 @@
   </si>
   <si>
     <t>assign</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>VISITA</t>
+  </si>
+  <si>
+    <t>data("VISITA") != "2"</t>
+  </si>
+  <si>
+    <t>Is anybody home?</t>
+  </si>
+  <si>
+    <t>Está alguém em casa?</t>
+  </si>
+  <si>
+    <t>end if</t>
+  </si>
+  <si>
+    <t>List of persons</t>
+  </si>
+  <si>
+    <t>Lista de pessoas</t>
+  </si>
+  <si>
+    <t>Tabz: {{data.TABZ}}</t>
+  </si>
+  <si>
+    <t>Camo: {{data.CAMO}}</t>
+  </si>
+  <si>
+    <t>House: {{data.CAMO}}</t>
+  </si>
+  <si>
+    <t>Grupo: {{data.HOUSEGRP}}</t>
+  </si>
+  <si>
+    <t>Family: {{data.FAM}}</t>
+  </si>
+  <si>
+    <t>House group: {{data.HOUSEGRP}}</t>
+  </si>
+  <si>
+    <t>Familia: {{data.FAM}}</t>
+  </si>
+  <si>
+    <t>Group in study: {{data.RANGROUP}}</t>
+  </si>
+  <si>
+    <t>Grupo de estudo: {{data.RANGROUP}}</t>
   </si>
 </sst>
 </file>
@@ -1006,11 +1039,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3:G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,10 +1106,10 @@
         <v>37</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1089,10 +1122,10 @@
         <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="H3" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1100,10 +1133,10 @@
         <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1111,10 +1144,10 @@
         <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>120</v>
+        <v>159</v>
       </c>
       <c r="H5" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1122,10 +1155,10 @@
         <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="H6" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1133,21 +1166,21 @@
         <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="H7" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1165,7 +1198,7 @@
         <v>30</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s">
         <v>47</v>
@@ -1176,19 +1209,19 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" t="s">
         <v>62</v>
-      </c>
-      <c r="E12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1206,67 +1239,34 @@
         <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" t="s">
-        <v>114</v>
+        <v>57</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="H15" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" t="s">
-        <v>115</v>
-      </c>
-      <c r="H16" t="s">
-        <v>109</v>
+      <c r="B16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" t="s">
-        <v>116</v>
-      </c>
-      <c r="H17" t="s">
-        <v>107</v>
+      <c r="B17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" t="s">
-        <v>117</v>
-      </c>
-      <c r="H18" t="s">
-        <v>110</v>
+      <c r="B18" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
@@ -1274,51 +1274,136 @@
         <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="G19" t="s">
         <v>113</v>
       </c>
       <c r="H19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>39</v>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>38</v>
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>142</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>143</v>
+        <v>58</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="G22" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="H22" t="s">
-        <v>50</v>
-      </c>
-      <c r="N22" t="b">
-        <v>1</v>
-      </c>
-      <c r="O22" t="b">
-        <v>1</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>39</v>
+      </c>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E28" t="s">
+        <v>137</v>
+      </c>
+      <c r="G28" t="s">
+        <v>152</v>
+      </c>
+      <c r="H28" t="s">
+        <v>153</v>
+      </c>
+      <c r="N28" t="b">
+        <v>1</v>
+      </c>
+      <c r="O28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1333,7 +1418,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,114 +1445,114 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1475,72 +1560,77 @@
     </row>
     <row r="11" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11">
+        <v>60</v>
+      </c>
+      <c r="B11" t="str">
+        <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12">
+        <v>60</v>
+      </c>
+      <c r="B12" t="str">
+        <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13">
+        <v>60</v>
+      </c>
+      <c r="B13" t="str">
+        <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="12">
+        <v>60</v>
+      </c>
+      <c r="B14" t="str">
+        <f>"4"</f>
         <v>4</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15">
+        <v>60</v>
+      </c>
+      <c r="B15" t="str">
+        <f>"5"</f>
         <v>5</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1551,72 +1641,77 @@
     </row>
     <row r="17" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17">
+        <v>59</v>
+      </c>
+      <c r="B17" t="str">
+        <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="12">
+        <v>59</v>
+      </c>
+      <c r="B18" t="str">
+        <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="12">
+        <v>59</v>
+      </c>
+      <c r="B19" t="str">
+        <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21">
+        <v>57</v>
+      </c>
+      <c r="B21" t="str">
+        <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="10">
+        <v>57</v>
+      </c>
+      <c r="B22" t="str">
+        <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1624,58 +1719,62 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24">
+        <v>58</v>
+      </c>
+      <c r="B24" t="str">
+        <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25">
+        <v>58</v>
+      </c>
+      <c r="B25" t="str">
+        <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26">
+        <v>58</v>
+      </c>
+      <c r="B26" t="str">
+        <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27">
+        <v>58</v>
+      </c>
+      <c r="B27" t="str">
+        <f>"4"</f>
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2013,54 +2112,54 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2071,11 +2170,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C6"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,10 +2202,10 @@
     </row>
     <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C2" s="10" t="b">
         <v>0</v>
@@ -2114,10 +2213,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C3" s="3" t="b">
         <v>0</v>
@@ -2126,10 +2225,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C4" s="3" t="b">
         <v>0</v>
@@ -2138,10 +2237,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C5" s="3" t="b">
         <v>0</v>
@@ -2150,10 +2249,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C6" s="3" t="b">
         <v>0</v>
@@ -2162,16 +2261,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2179,7 +2278,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>30</v>
@@ -2190,56 +2289,56 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>127</v>
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
       </c>
       <c r="C10" s="3" t="b">
         <v>0</v>
       </c>
       <c r="I10" s="10"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="3" t="b">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>126</v>
+        <v>49</v>
       </c>
       <c r="C13" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>126</v>
+        <v>49</v>
       </c>
       <c r="C14" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>126</v>
+        <v>49</v>
       </c>
       <c r="C15" s="3" t="b">
         <v>0</v>
@@ -2247,40 +2346,51 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>126</v>
+        <v>49</v>
       </c>
       <c r="C16" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I17" s="10"/>
+      <c r="A17" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C18" s="3" t="b">
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I20" s="10"/>
+      <c r="D19" s="3" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I21" s="10"/>
     </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="10"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I8:I24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I8:I25">
     <sortCondition ref="I8"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Updates to inclusion after field trip
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKHOUSEHOLD/Forms/MASKHOUSEHOLD/MASKHOUSEHOLD.xlsx
+++ b/app/config/tables/MASKHOUSEHOLD/Forms/MASKHOUSEHOLD/MASKHOUSEHOLD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B9A3CC-8DBA-41D5-820B-8D496B0FEADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424BA514-7157-4375-A854-25380FBC89B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="168">
   <si>
     <t>setting_name</t>
   </si>
@@ -523,6 +523,21 @@
   </si>
   <si>
     <t>Grupo de estudo: {{data.RANGROUP}}</t>
+  </si>
+  <si>
+    <t>OID</t>
+  </si>
+  <si>
+    <t>KEL</t>
+  </si>
+  <si>
+    <t>Odies</t>
+  </si>
+  <si>
+    <t>Oides</t>
+  </si>
+  <si>
+    <t>Kelbit</t>
   </si>
 </sst>
 </file>
@@ -1041,7 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
@@ -1414,11 +1429,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D104"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,51 +1571,49 @@
       </c>
     </row>
     <row r="10" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C10"/>
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="11" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>79</v>
+        <v>52</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>167</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>94</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>95</v>
-      </c>
+      <c r="C12"/>
     </row>
     <row r="13" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
       <c r="B13" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>81</v>
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1608,14 +1621,14 @@
         <v>60</v>
       </c>
       <c r="B14" t="str">
-        <f>"4"</f>
-        <v>4</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>82</v>
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1623,143 +1636,143 @@
         <v>60</v>
       </c>
       <c r="B15" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="str">
         <f>"5"</f>
         <v>5</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C17" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D17" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-    </row>
-    <row r="17" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+    </row>
+    <row r="19" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>59</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B19" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>84</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B20" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D20" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>59</v>
       </c>
-      <c r="B19" t="str">
+      <c r="B21" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D21" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>57</v>
       </c>
-      <c r="B21" t="str">
+      <c r="B23" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>86</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>57</v>
       </c>
-      <c r="B22" t="str">
+      <c r="B24" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>87</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" t="s">
-        <v>102</v>
-      </c>
-    </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" t="s">
-        <v>103</v>
-      </c>
+      <c r="A25" s="12"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>58</v>
       </c>
       <c r="B26" t="str">
-        <f>"3"</f>
-        <v>3</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1767,31 +1780,51 @@
         <v>58</v>
       </c>
       <c r="B27" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>93</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D29" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-    </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
+      <c r="B30" s="7"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
+      <c r="B31" s="7"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
@@ -1894,34 +1927,37 @@
       <c r="D51" s="13"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="7"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="7"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="7"/>
-      <c r="C55" s="13"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
       <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
+      <c r="C57" s="13"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
+      <c r="C58" s="13"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
@@ -1929,7 +1965,6 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="7"/>
@@ -1940,7 +1975,7 @@
       <c r="C63" s="7"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="15"/>
+      <c r="B64" s="7"/>
       <c r="C64" s="7"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
@@ -1948,7 +1983,7 @@
       <c r="C65" s="7"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="7"/>
+      <c r="B66" s="15"/>
       <c r="C66" s="7"/>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
@@ -2017,21 +2052,23 @@
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="7"/>
-      <c r="C83" s="15"/>
+      <c r="C83" s="7"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="7"/>
       <c r="C85" s="15"/>
-      <c r="D85" s="15"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="7"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="7"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="15"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="7"/>
@@ -2083,6 +2120,12 @@
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="7"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105" s="7"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Updates to FU and incl in office
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKHOUSEHOLD/Forms/MASKHOUSEHOLD/MASKHOUSEHOLD.xlsx
+++ b/app/config/tables/MASKHOUSEHOLD/Forms/MASKHOUSEHOLD/MASKHOUSEHOLD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC668D38-33DF-4DC2-B721-AAE12D0A6607}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206C9522-2E48-4D12-A384-9A9B4EA407FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="167">
   <si>
     <t>setting_name</t>
   </si>
@@ -468,12 +468,6 @@
     <t>display.hide_add_instance</t>
   </si>
   <si>
-    <t>adate.today()</t>
-  </si>
-  <si>
-    <t>assign</t>
-  </si>
-  <si>
     <t>if</t>
   </si>
   <si>
@@ -535,6 +529,12 @@
   </si>
   <si>
     <t>Kelbit</t>
+  </si>
+  <si>
+    <t>Missing information</t>
+  </si>
+  <si>
+    <t>Falta informação</t>
   </si>
 </sst>
 </file>
@@ -1051,11 +1051,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,10 +1134,10 @@
         <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1145,10 +1145,10 @@
         <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1156,10 +1156,10 @@
         <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1167,10 +1167,10 @@
         <v>46</v>
       </c>
       <c r="G6" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" t="s">
         <v>158</v>
-      </c>
-      <c r="H6" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1178,107 +1178,113 @@
         <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" t="s">
-        <v>144</v>
+      <c r="B8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>38</v>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>30</v>
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" t="s">
-        <v>62</v>
+      <c r="B12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="H15" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>39</v>
+        <v>144</v>
+      </c>
+      <c r="C16" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C17" t="s">
-        <v>148</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>38</v>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
@@ -1286,16 +1292,16 @@
         <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
@@ -1303,16 +1309,16 @@
         <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
@@ -1320,102 +1326,85 @@
         <v>49</v>
       </c>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H21" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" t="s">
-        <v>58</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G22" t="s">
-        <v>116</v>
-      </c>
-      <c r="H22" t="s">
-        <v>109</v>
-      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24" t="s">
+        <v>112</v>
+      </c>
+      <c r="H24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>39</v>
-      </c>
-      <c r="F23" s="10"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="10"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="G25" t="s">
-        <v>112</v>
-      </c>
-      <c r="H25" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>136</v>
+      </c>
+      <c r="E27" t="s">
+        <v>137</v>
+      </c>
+      <c r="G27" t="s">
+        <v>150</v>
+      </c>
+      <c r="H27" t="s">
+        <v>151</v>
+      </c>
+      <c r="N27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>136</v>
-      </c>
-      <c r="E28" t="s">
-        <v>137</v>
-      </c>
-      <c r="G28" t="s">
-        <v>152</v>
-      </c>
-      <c r="H28" t="s">
-        <v>153</v>
-      </c>
-      <c r="N28" t="b">
-        <v>1</v>
-      </c>
-      <c r="O28" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1426,11 +1415,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,13 +1561,13 @@
         <v>52</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>165</v>
-      </c>
       <c r="D10" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1586,13 +1575,13 @@
         <v>52</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>166</v>
-      </c>
       <c r="D11" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1674,236 +1663,279 @@
       </c>
     </row>
     <row r="18" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="str">
+        <f>"9"</f>
+        <v>9</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="19" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" t="s">
-        <v>99</v>
-      </c>
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
     </row>
     <row r="20" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
       <c r="B20" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D21" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>59</v>
       </c>
-      <c r="B21" t="str">
+      <c r="B22" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C22" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D22" s="12" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="str">
+        <f>"9"</f>
+        <v>9</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>57</v>
       </c>
-      <c r="B23" t="str">
+      <c r="B25" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
         <v>86</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>57</v>
       </c>
-      <c r="B24" t="str">
+      <c r="B26" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>87</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D26" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>90</v>
-      </c>
-      <c r="D26" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" t="s">
-        <v>103</v>
+        <f>"9"</f>
+        <v>9</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" t="s">
-        <v>104</v>
-      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>58</v>
       </c>
       <c r="B29" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C32" t="s">
         <v>93</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D32" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" t="str">
+        <f>"9"</f>
+        <v>9</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
@@ -1934,34 +1966,38 @@
       <c r="D53" s="13"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="7"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="7"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="7"/>
+      <c r="B56" s="13"/>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="7"/>
-      <c r="C57" s="13"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
-      <c r="C58" s="13"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
+      <c r="C60" s="13"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
+      <c r="C61" s="13"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="7"/>
@@ -1973,14 +2009,13 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="15"/>
+      <c r="B66" s="7"/>
       <c r="C66" s="7"/>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
@@ -1992,7 +2027,7 @@
       <c r="C68" s="7"/>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="7"/>
+      <c r="B69" s="15"/>
       <c r="C69" s="7"/>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
@@ -2057,24 +2092,27 @@
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="7"/>
-      <c r="C85" s="15"/>
+      <c r="C85" s="7"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="7"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="15"/>
+      <c r="C87" s="7"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="7"/>
+      <c r="C88" s="15"/>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="7"/>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="7"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="15"/>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="7"/>
@@ -2123,6 +2161,15 @@
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="7"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107" s="7"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108" s="7"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -2341,7 +2388,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Small update to counting in INCL
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKHOUSEHOLD/Forms/MASKHOUSEHOLD/MASKHOUSEHOLD.xlsx
+++ b/app/config/tables/MASKHOUSEHOLD/Forms/MASKHOUSEHOLD/MASKHOUSEHOLD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6506D4B-24E5-44BB-9D15-5DBDFEE1C8CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DE7F17-9D30-42EE-8AD0-E9BCE1C64EA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="728" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -1075,9 +1075,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,6 +1228,9 @@
       </c>
       <c r="H10" t="s">
         <v>48</v>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2604,7 +2607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B196E6E-CD9E-4642-805B-A176E472060D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>